<commit_message>
Scrap iphone 11 data from Kijiji website for details!!!
</commit_message>
<xml_diff>
--- a/products.xlsx
+++ b/products.xlsx
@@ -460,29 +460,29 @@
       <c r="A2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 . Brand New. 64g unlocked
+                            DESIGNER phone case DESIGNERS all APPLE all SAMSUNG 647-874-1414
 </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $850.00
+                                     Please Contact
                     </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Downtown-West End
-12/09/2020
+                            Mississauga / Peel Region
+25/08/2020
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Neeeeww Iphone 11 never used 64g Unlocked Still in the box Text me or call me : 438-506-6142. ONLY CASH
+                        DESIGNER PHONE CASES STARTING FROM $15.00and up! ⭐️LOTS OF DESIGNER CASES FOR IPHONE X, IPHONE XS, IPHONE XR, IPHONE 11, IPHONE 11 PRO AND IPHONE 11 PRO MAX. LOTS OF DESIGNS TO CHOOSE FROM. ⭐️ ...
 </t>
         </is>
       </c>
@@ -491,29 +491,30 @@
       <c r="A3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Cash for iPhones in any Condition $$$
+                            Wanted:
+                            I will BUY your PHONE for Cash Right Now!
 </t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $999.00
-                    </t>
+                                    $77,777.00
+</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Edmonton
-04/09/2020
+                            Markham / York Region
+25/08/2020
 </t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        We offer same day quick cash for your iPhone. The phone can be in any condition as long as it turns on so we can test it. ***WE WILL NOT BUY BLACKLISTED, ICLOUD LOCKED, OR WATER DAMAGED IPHONES*** ...
+                        iPhone SE 6s 7 8 X XR Xs 11 Pro Max Plus 64GB 256GB 128GB 32GB 512GB 16GB Samsung s7 s8 s9 s10 S20 + Ultra A50 A70 A71 Note 9 10 iPad Pro Air Mini 10.5 12.9 11 Inch 2nd 3rd 4th 6th 7th Gen Series 3 4 ...
 </t>
         </is>
       </c>
@@ -522,29 +523,29 @@
       <c r="A4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            ✅Appelé Broski ✅J'achète iPhone 11 Pro Max Samsung Pixel Macbook
+                            Brand New &amp; Unlocked iPhone-11 ProMax,11-Pro &amp; iPhone-11 &amp; SE-2
 </t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $99,999.00
+                                    $550.00
                     </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Montréal
-23/07/2020
+                            Oshawa / Durham Region
+10/09/2020
 </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        J’ACHETE I BUY TOUT LES IPHONE SAMSUNG GOOGLE PIXEL IPAD IPAD PRO MACBOOK PRO MACBOOK AIR IMAC NEUF SEULEMENT NEW ONLY SURFACE PRO 4 SURFACE BOOK APELLER MTN BROSKI 514-512-0292 514-512-0292 SEALED ...
+                        We're selling following Brand New &amp; Unlocked iPhone-11 &amp; SE-2 phones; iPhone SE-2nd Gen, 64GB (New) With Charger only in $550 ----------------------------------- iPhone SE-2nd Gen, 128GB (New) With ...
 </t>
         </is>
       </c>
@@ -553,29 +554,29 @@
       <c r="A5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand New &amp; Unlocked iPhone-11 ProMax,11-Pro &amp; iPhone-11 &amp; SE-2
+                            iPhone 11 Pro Max gold sealed BEWARE
 </t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $550.00
+                                    $1,200.00
                     </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Oshawa / Durham Region
-10/09/2020
+                            City of Toronto
+19/08/2020
 </t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        We're selling following Brand New &amp; Unlocked iPhone-11 &amp; SE-2 phones; iPhone SE-2nd Gen, 64GB (New) With Charger only in $550 ----------------------------------- iPhone SE-2nd Gen, 128GB (New) With ...
+                        BEWARE , i met up with someone and gave them $1200 cash for a fake iphone. MAKE sure you open sealed case in front of seller before handing cash because this seller had legitimate receipt with IMEI ...
 </t>
         </is>
       </c>
@@ -584,29 +585,29 @@
       <c r="A6" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            IPHONE REPAIR SPECIALIST @UNBEATABLE PRICE
+                            iPhone 11 Pro 64 GB Space Gray [SEALED]
 </t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $35.00
+                                    $1,325.00
                     </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-11/09/2020
+                            City of Toronto
+09/09/2020
 </t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        CELLUCOM ELECTRONICS INC 808 Britannia road west (Unit 102) Call : (905) 826 9737 Timing Monday to Friday : 10AM - 7PM Saturday : 11AM - 6PM Apple iPhone 8/8+ screen repair $80 Apple iPhone 7 screen ...
+                        iPhone 11 Pro 64 GB Space Gray. Got it through carrier upgrade but already have the same phone from before. The Phone is FULLY unlocked, will work with any service provider. It has not been turned ...
 </t>
         </is>
       </c>
@@ -615,29 +616,29 @@
       <c r="A7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            I phone 11
+                            iPhone 11 
 </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $950.00
+                                    $800.00
                     </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-11/09/2020
+                            Laval / North Shore
+&lt; 3 minutes ago
 </t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Hello! Selling beauitful iPhone 11 limited edition lavender colour. This phone is from apple in box with charger, 64GB Thanks!
+                        iPhone 11 64gb new sealed 800$ no nego aplle au 5148028587
 </t>
         </is>
       </c>
@@ -646,29 +647,29 @@
       <c r="A8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11
+                            iPhone 11 Pro 64gb Mint Space Grey
 </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $950.00
+                                    $1,200.00
                     </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-10/09/2020
+                            Ottawa
+&lt; 3 minutes ago
 </t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        iPhone 11 Unopened box White 64 GB
+                        Comes with charger, screen protector and a case Mint condition, no scratches or marks Fully unlocked and supports eSim No icloud account fully reset Selling for 1200$ Available at Allo Allo Wireless ...
 </t>
         </is>
       </c>
@@ -677,14 +678,14 @@
       <c r="A9" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 
+                            iPhone SE 6 6S 7 7PLUS 8 8PLUS X XS MAX XR 11 PRO MAX
 </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $800.00
+                                    $150.00
                     </t>
         </is>
       </c>
@@ -692,14 +693,14 @@
         <is>
           <t xml:space="preserve">
                             Hamilton
-11/09/2020
+&lt; 3 minutes ago
 </t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Iphone 11 for sale Good condition no cracks Still under warranty No box Need gone fast
+                        Buy with confidence from Limeridge mall (Hamilton). Our kiosk (booth) is located in front of Hudson's Bay Store upper level (2nd level) of mall. I TECH ACCESSORIES.289-489-9786 Starting price is ...
 </t>
         </is>
       </c>
@@ -708,14 +709,14 @@
       <c r="A10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11
+                            Brand New Sealed Iphone 11 Unlocked
 </t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,020.00
+                                    $850.00
                     </t>
         </is>
       </c>
@@ -723,14 +724,14 @@
         <is>
           <t xml:space="preserve">
                             City of Toronto
-&lt; 23 hours ago
+&lt; 5 minutes ago
 </t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        -BNIB Unlocked iPhone 11 Black 128gb -Comes with a glass screen protector
+                        Brand New Sealed IPhone 11 Unlocked 64g Blade. Price $850. Call 416 817 8365
 </t>
         </is>
       </c>
@@ -739,29 +740,29 @@
       <c r="A11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand new iPhone 11
+                            iPhone 11Pro MAX 64GB like new 
 </t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $920.00
+                                    $1,300.00
                     </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-&lt; 23 hours ago
+                            City of Montréal
+&lt; 6 minutes ago
 </t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        iPhone 11 Brand new sealed in box With carrier: Virgin/ Bell 64 gb
+                        Warranty unit AUGUST 2021
 </t>
         </is>
       </c>
@@ -770,28 +771,28 @@
       <c r="A12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 Pro 64 GB Green Unlocked -- Buy from a trusted source (with 5-star customer service!)
+                            Google pixel  XL brand new for $149 , 173 montreal road , Ottawa ,
 </t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-         $1,105.00
-</t>
+         $139.00
+                    </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
+                            Ottawa
 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        **New in stock! This handset is unlocked and can be used with any carrier.** We guarantee that it will work just like new and back that with a 90 day no-questions-asked returns policy (and free return shipping) not to mention a lifetime blacklist guarantee! Condition: its external appearance shows some wear and
+                        OTTAWA CELLPHONES OFFER AMAZING DEALS , BUY WITH CONFIDENCE , WE BEAT ALL PRICES, GOOGLE PIXEL XL $149 brand new LOTS MORE PLEASE VISIT FOR ALL MODELS OF SAMSUNG , IPHONES , LG, MOTOROLLA , ZTE ,ETC.. 173 MONTREAL RD. VANIER , OTTAWA , K1L6E4, 6136955005 WE ARE INSIDE chatr store, AT INTERSECTION OF VANIER PARKWAY
 </t>
         </is>
       </c>
@@ -800,29 +801,29 @@
       <c r="A13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 128gb Black
+                            Iphone 8 &amp; 8 plus Iphone X &amp; XR Iphone 11 with Warranty for sale
 </t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $950.00
+                                    $700.00
                     </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Oakville / Halton Region
-&lt; 20 hours ago
+                            Hamilton
+&lt; 6 minutes ago
 </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Selling a pristine condition iphone 11 128gb. Phone was purchased directly from Apple. Receipt can be provided for proof. Phone was used in a case 100% of the time. - 100% battery health - warranty ...
+                        Phones are unlocked and comes with 6 months warranty. We add free case and glass screen protector with every phone. Iphone 8 64 gigs $425 Iphone 8 plus 64 gigs $550 Iphone X 64 gigs $700 Iphone XR 64 ...
 </t>
         </is>
       </c>
@@ -831,29 +832,29 @@
       <c r="A14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 Black 64 GB - BNIB!
+                            ✔️Reparation Batterie &amp; Écran LCD iPhone 11 XS MAX XR XS 8+
 </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $950.00
+                                    $30.00
                     </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-10/09/2020
+                            City of Montréal
+&lt; 9 minutes ago
 </t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new iPhone 11, 64 GB in black. Never opened, still sealed with full warranty and unlocked. Got it through plan upgrade.
+                        *** 514-277-7883 / 514-277-7883 *** 440 saint-roch montreal H3N 1K3 (Pres du metro parc) Lundi au vendredi : 10h am - 18h pm Samedi : 10h am - 17h pm / Dimanche Fermer ...
 </t>
         </is>
       </c>
@@ -862,29 +863,29 @@
       <c r="A15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Apple iPhone 11 pro max
+                            IPHONE REPAIR SPECIALIST @UNBEATABLE PRICE
 </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,300.00
+                                    $35.00
                     </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Winnipeg
-12/09/2020
+                            Mississauga / Peel Region
+&lt; 16 minutes ago
 </t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        This a lightly used iPhone 11 Pro Max. Color is Midnight Green and it is 64 GB version. Included is every piece of accessory/ box plus a clear case. The phone is Totally Mint condition.. 1350 firm. ...
+                        CELLUCOM ELECTRONICS INC 808 Britannia road west (Unit 102) Call : (905) 826 9737 Timing Monday to Friday : 10AM - 7PM Saturday : 11AM - 6PM Apple iPhone 8/8+ screen repair $80 Apple iPhone 7 screen ...
 </t>
         </is>
       </c>
@@ -893,29 +894,29 @@
       <c r="A16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            BRAND NEW Unopened iPhone 11
+                            “Store Clearance” Biggest sale Brand New Sealed Iphone 11 Black
 </t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $950.00
+                                    $890.00
                     </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-07/09/2020
+                            Mississauga / Peel Region
+&lt; 17 minutes ago
 </t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new 64 GB
+                        “Store Clearance” Biggest sale Brand New Sealed Iphone 11 Black 64gb 1 year apple warranty Shiza Cellular and Electronics Located at Westwood Square Mall Mississuga Address 7215 Goreway Dr, unit # ...
 </t>
         </is>
       </c>
@@ -924,29 +925,29 @@
       <c r="A17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            brand new iphone 11
+                            “Store Clearance” Biggest sale Brand New  Sealed Apple Iphone 11
 </t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $900.00
+                                    $1,049.00
                     </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-12/09/2020
+                            Mississauga / Peel Region
+&lt; 17 minutes ago
 </t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new iPhone 11 for sale This phone has 64 gb of memory The phone is sealed in the original box. Never opened. The phone is linked with the following phone carriers: Virgin &amp; Bell
+                        “Store Clearance” Biggest sale Brand New Sealed Apple Iphone 11 Black 128gb 1 year apple warrantyShiza Cellular and Electronics Located at Westwood Square Mall Mississuga Address 7215 Goreway Dr, ...
 </t>
         </is>
       </c>
@@ -955,29 +956,29 @@
       <c r="A18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 Apple silicone case
+                            NEW IPHONE     11     64GB UNLOCKED BLK/RED/PURPLE
 </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $15.00
+                                    $899.00
                     </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Kitchener / Waterloo
-04/09/2020
+                            Mississauga / Peel Region
+&lt; 21 minutes ago
 </t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Ad says it all! Black Apple silicone case for the iPhone 11, brand new and in sealed packaging. 15$ Firm (I think this case is still very expensive in stores)
+                        THIS LISTING IS FOR NEW IPHONE 11 64GB UNLOCKED BLK/RED/PURPLE BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA ********************************************************************** VAUGHAN MILLS ...
 </t>
         </is>
       </c>
@@ -1016,30 +1017,29 @@
       <c r="A20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Wanted:
-                            Looking for mint condition iPhone 11, 11 Pro, 11 Pro Max!!!
+                            NEW  IPHONE 11 PRO 64GB UNLOCKED BLACK
 </t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $8,888.00
+                                    $1,249.95
                     </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-05/09/2020
+                            Mississauga / Peel Region
+&lt; 22 minutes ago
 </t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Looking to buy brand new or mint condition 10/10 iPhone 11, 11 Pro, 11 Pro Max any color, I would pay cash for it only right away! Please contact me by text message or email if you have one for sale!
+                        THIS LISTIN G IS FOR NEW IPHONE 11 PRO 64GB UNLOCK ED BLA CK *************************************************************** BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA - ...
 </t>
         </is>
       </c>
@@ -1048,29 +1048,29 @@
       <c r="A21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand New Sealed iphone 11 64GB Green
+                            NEW SEALED IPHONE  11     64GB BLACK UNLOCKED
 </t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $970.00
+                                    $899.00
                     </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Barrie
-31/08/2020
+                            Markham / York Region
+&lt; 26 minutes ago
 </t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand New Sealed iphone 11 64GB Memory Green colour available Unlocked With any carrier Comes with 1 year apple warranty buy worry free!!!
+                        THIS LISTING IS FOR NEW SEA LED IPHONE 11 64GB BLACK UNLOCKED *************************************************************** BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA - ...
 </t>
         </is>
       </c>
@@ -1079,29 +1079,29 @@
       <c r="A22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand New iPhone 11 - 64 GB White
+                            iPhone 11 Pro Max 512gb 
 </t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $935.00
+                                    $2,000.00
                     </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-08/09/2020
+                            City of Toronto
+&lt; 26 minutes ago
 </t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        I bought a brand new 64 GB White iPhone 11 from Freedom Mobile around 3 Weeks back (under contract). However, I have a better offer from Bell now. Hence I am selling this phone to end my contract ...
+                        For sale I have a Brand new sealed IPhone 11 Pro Max 512gb space grey . NO TIME WASTERS IF YOU HAVE THE CASH MESSAGE ME , NO LOW BALLERS I Price is 2000.00 you save the tax 300$
 </t>
         </is>
       </c>
@@ -1110,14 +1110,14 @@
       <c r="A23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            NEW SEALED IPHONE   11 64GB UNLOCKED BLACK
+                            Iphone 11 pro 64gb army green
 </t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $899.00
+                                    $1,100.00
                     </t>
         </is>
       </c>
@@ -1125,14 +1125,14 @@
         <is>
           <t xml:space="preserve">
                             Markham / York Region
-&lt; 10 minutes ago
+&lt; 28 minutes ago
 </t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        THIS LISTING IS FOR NEW SEA LED IPHONE 11 64GB UNLOCKED BLACK *************************************************************** BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA ...
+                        Looking to cell because im switching back to android. Has been in a case since the day i bought it
 </t>
         </is>
       </c>
@@ -1141,29 +1141,29 @@
       <c r="A24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            NEW   SEALED IPHONE  11 64GB BLK/PURPLE/RED
+                            BUYING ALL CRACKED/ BROKEN IPHONE 11- X - Xs - Xr - 8
 </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $899.00
+                                    $480.00
                     </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-&lt; 4 minutes ago
+                            City of Toronto
+&lt; 29 minutes ago
 </t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        THIS LISTING IS FOR NEW SEALED IPHONE 11 64GB BLK/PURPLE/RED *************************************************************** BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA - ...
+                        |(647) 274-9382| I'm buying all cracked/ broken IPhone X/ Xr / XS and up regardless of its condition, only requirements is that they are in working order and not stolen. Buying ; -Iphone 8+ -Iphone X ...
 </t>
         </is>
       </c>
@@ -1172,29 +1172,29 @@
       <c r="A25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand New Sealed iphone 11 64GB Purple
+                            ✔️✅Réparation cellulaire à Petit Prix iPhone Samsung✔️+Garantie✅
 </t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $970.00
+                                    $29.00
                     </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Barrie
-31/08/2020
+                            City of Montréal
+&lt; 29 minutes ago
 </t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand New Sealed iphone 11 64GB Memory Purple colour available Unlocked With any carrier Comes with 1 year apple warranty buy worry free!!!
+                        repair lcd vitre cassé batterie battery remplacement water damage eau liquide iPhone 11 pro SE max xs 8 6S 5S 7 Plus samsung s4 S5 S6 S7 S8 S9 S20 ultra LG G3 G4 G5 G6 iPad Mini Pro Air ps4 s10 plus ...
 </t>
         </is>
       </c>
@@ -1203,14 +1203,14 @@
       <c r="A26" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            BRAND NEW SEALED IPHONE 11 64GB WITH EARPODS.
+                            APPLE IPHONE 11 PRO 64GB / 256GB / 512GB
 </t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $850.00
+                                    $1,149.00
                     </t>
         </is>
       </c>
@@ -1218,14 +1218,14 @@
         <is>
           <t xml:space="preserve">
                             City of Toronto
-07/09/2020
+&lt; 30 minutes ago
 </t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        *IF ADD IS STILL UP, PHONE IS AVAILABLE* ***PRICE IS $850 FIRM*** Don't waste your time trying to haggle and negotiate! Brand new, never used iPhone 11 64GB (black) for sale. Phone is unlocked and ...
+                        CERTIFIED PREOWNED WITH AROUND 4-6 MONTH APPLE WARRANTY ☆☆ APPLE IPHONE 11 PRO 64GB - $1150 APPLE IPHONE 11 PRO 256GB - $1350 APPLE IPHONE 11 PRO 512GB - $1500 ☆☆ Midnight Green Silver Space grey ...
 </t>
         </is>
       </c>
@@ -1234,29 +1234,29 @@
       <c r="A27" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Buying ✔✅ acheter IPHONE XR XMAX ✔ IPHONE 11 PRO ✔ SAMSUNG ✔ CAL
+                            128GB iPhone 11 Brand New Sealed Box -Warranty
 </t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,900.00
+                                    $980.00
                     </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Montréal
-12/09/2020
+                            City of Toronto
+&lt; 30 minutes ago
 </t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        ✅ ps4 xbox dyson v11 v10 Iphone 11 pro max x xs 64gb 128gb macbook playstation ps4 xbox imac pro air ipad samsung S9 note 9 s8 s7 s5 huwaei p20 pro lg g3 g4 g5 g7 ✅✅✅ (438) 8333 932 ✅✅✅ APEL ...
+                        128GB iPhone 11 Brand new Sealed in box. Retails for 1300$ with tax. Never used with one year warranty. Unlocked sealed Call or text only 647 849 9759 Unlocked to work with any service provider ...
 </t>
         </is>
       </c>
@@ -1265,29 +1265,29 @@
       <c r="A28" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand New Iphone 11 64gb
+                            Iphone 11
 </t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $925.00
+                                    $800.00
                     </t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-&lt; 22 hours ago
+                            Calgary
+&lt; 32 minutes ago
 </t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new sealed Apple iphone 11 64gb (Black). Comes with full 1 year Apple warranty and eligable for Apple care plus. Located in Mississauga.
+                        Iphone 11 new in the box selling for 800$ only black color 64 gb no low ballers!
 </t>
         </is>
       </c>
@@ -1296,29 +1296,29 @@
       <c r="A29" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 64GB New
+                            SAMSUNG S20 ULTRA 128GB UNLOCKED ✅ BRAND NEW / NEUF
 </t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                     Please Contact
+                                    $1,350.00
                     </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-07/09/2020
+                            City of Montréal
+&lt; 33 minutes ago
 </t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        iPhone 11 64GB New in box All accessories receipt of payment price negotiable
+                        SAMSUNG S20 ULTRA 128GB GREY BRAND NEW in the BOX / NEUF DANS LA BOITE 1 YEAR SAMSUNG WARRANTY CALL 438 988 5597 FIRM PRICE
 </t>
         </is>
       </c>
@@ -1327,30 +1327,29 @@
       <c r="A30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Wanted:
-                            looking for Iphone 11 128gb!!
+                            SAMSUNG S20 PLUS 128GB UNLOCKED WITH THE BILL ✅ SEALED / SCELLÉ
 </t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                     Please Contact
+                                    $1,000.00
                     </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-02/09/2020
+                            City of Montréal
+&lt; 35 minutes ago
 </t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        I’m looking for an iphone 11 128gb with a battery capacity above 95.
+                        SAMSUNG S20+ 128GB COSMIC BLACK BRAND NEW in the BOX SEALED / NEUF DANS LA BOITE SCELLEE 1 YEAR SAMSUNG WARRANTY AVEC LA FACTURE / WITH THE BILL CALL 438 988 5597 FIRM PRICE
 </t>
         </is>
       </c>
@@ -1359,14 +1358,14 @@
       <c r="A31" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 pro gold 64
+                            iPhone 11 black brand new sealed 
 </t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,200.00
+                                    $950.00
                     </t>
         </is>
       </c>
@@ -1374,14 +1373,14 @@
         <is>
           <t xml:space="preserve">
                             City of Toronto
-05/09/2020
+&lt; 35 minutes ago
 </t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Selling BNIB iphone 11 pro gold 64gb unlocked and with 1 year warranty
+                        iPhone 11 256GB brand new sealed in box
 </t>
         </is>
       </c>
@@ -1390,28 +1389,28 @@
       <c r="A32" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Google pixel  XL brand new for $149 , 173 montreal road , Ottawa ,
+                            Buying all IPhones and Samsung products
 </t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
           <t xml:space="preserve">
-         $139.00
+         $9,999.00
                     </t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Ottawa
+                            Mississauga / Peel Region
 </t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        OTTAWA CELLPHONES OFFER AMAZING DEALS , BUY WITH CONFIDENCE , WE BEAT ALL PRICES, GOOGLE PIXEL XL $149 brand new LOTS MORE PLEASE VISIT FOR ALL MODELS OF SAMSUNG , IPHONES , LG, MOTOROLLA , ZTE ,ETC.. 173 MONTREAL RD. VANIER , OTTAWA , K1L6E4, 6136955005 WE ARE INSIDE chatr store, AT INTERSECTION OF VANIER PARKWAY
+                        Get Cash for All Brand new Apple iPhones sealed/Unsealed Locked/unlocked For Cash! Also Buying all upgraded lines, personal lines and corporate lines as well ! Any quantity is welcome! Call or Text 647-719-7977 Any Carrier Original Sealed Box iPhone 6s 32gb - $150- 200 iPhone 7 32GB - $250-300 iPhone 7 128GB -
 </t>
         </is>
       </c>
@@ -1420,29 +1419,29 @@
       <c r="A33" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 . Brand New. 64g unlocked
+                            iPhone 11 64Gb New Unused Open Box Unlocked 
 </t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $850.00
+                                    $860.00
                     </t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Downtown-West End
-12/09/2020
+                            Mississauga / Peel Region
+&lt; 36 minutes ago
 </t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Neeeeww Iphone 11 never used 64g Unlocked Still in the box Text me or call me : 438-506-6142. ONLY CASH
+                        iPhone 11 64gb black unlocked New unused open box Comes with box and new unused accessories Phone still has seal on not unused battery health 100% and warranty until September 9, 2021 This is $1106 ...
 </t>
         </is>
       </c>
@@ -1451,29 +1450,29 @@
       <c r="A34" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            IPhone 11 black sealed box 64 gb 
+                            Apple iPhone XS 256GB! Like new in box!
 </t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $899.00
+                                    $725.00
                     </t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            London
-11/09/2020
+                            City of Toronto
+&lt; 36 minutes ago
 </t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new sealed never used Comes with one year warranty Never been out of box Happy to wait till you test your sim card before the purchase Price is firm and reasonable
+                        Selling a like brand new condition Apple iPhone XS 256GB Space Grey in original box. All accessories are new and never used. Priced to sell for only $725 OBO!
 </t>
         </is>
       </c>
@@ -1482,29 +1481,29 @@
       <c r="A35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Apple iPhone 11  - 256GB - Black (Unlocked) A2111 (CDMA +GSM) 
+                            MINT IPHONE 11 64GB UNLOCKED BLK
 </t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,050.00
+                                    $799.00
                     </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-&lt; 16 hours ago
+                            Markham / York Region
+&lt; 36 minutes ago
 </t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Condition is used. The screen was replaced on it at a local repair shop last month - screen has no scratches!! (Reason for replacement was a drop/ crack) Comes with Phone and Generic wall charger ...
+                        THIS LISTING IS FOR MINT IPHONE 11 64GB UNLOCKED BLK *************************************************************** BUY FROM A STORE BUY WITH CONFIDENCE BUYNCELL.CA ------------------------------ ...
 </t>
         </is>
       </c>
@@ -1513,29 +1512,29 @@
       <c r="A36" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 (IC Locked passcode locked)
+                            ✅ Réparation iPhone Rapide! Promo Lcd à 45$ ✅ garantie 90 Jours
 </t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                     Please Contact
+                                    $35.00
                     </t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Oshawa / Durham Region
-31/08/2020
+                            Laval / North Shore
+&lt; 37 minutes ago
 </t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Negotiable Comes with old screen but its cracked
+                        Phone repair broken screen lcd iPhone x 11 pro max xs 8 plus 5s 6 7 x Samsung note 10 plus s10 ipad air pro s4 s5 s6 s7 s8 lg g3 g4 g5 s6 s7 G3 G4 G5 samsung note 3 4 5 ✔️✔️✔️450 241-6313✔️✔️✔️ ...
 </t>
         </is>
       </c>
@@ -1544,29 +1543,29 @@
       <c r="A37" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone    11 pro 256gb with     warranty
+                            ✔️remplacement de Batterie et LCD iPhone en 10min ✔️✅Promo 29$
 </t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,225.00
+                                    $40.00
                     </t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Hamilton
-Yesterday
+                            Laval / North Shore
+&lt; 37 minutes ago
 </t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Selling an iPhone 11 pro 256gb in great condition. Warranty until June 2021. Phone only
+                        Phone repair broken screen lcd iPhone x 11 pro max xs 8 plus 5s 6 7 x Samsung note 10 plus s10 ipad air pro s4 s5 s6 s7 s8 lg g3 g4 g5 s6 s7 G3 G4 G5 samsung note 3 4 5 ✔️✔️✔️450 241-6313✔️✔️✔️ ...
 </t>
         </is>
       </c>
@@ -1575,29 +1574,29 @@
       <c r="A38" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            NEW SEALED IPHONE  11 64GB UNLOCKED  BLACK
+                            ✅✔️On Répare ton Lcd iphone X XR 109$ en 10min +Garantie 90jrs✅
 </t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $889.00
+                                    $30.00
                     </t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-Yesterday
+                            Laval / North Shore
+&lt; 37 minutes ago
 </t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        THIS LISTIN G IS FOR NEW SEA LED IPHONE 11 64GB UNLOCKED BLACK BUY FROM A STORE BUY WITH CONFIDENCE BUYNCELL.CA - ----------------------------- (ERIN MILLS N DUNDAS)MISSISSAUGA: (416) 840 7 005 1960 ...
+                        Phone repair broken screen lcd iPhone x 11 pro max xs 8 plus 5s 6 7 x Samsung note 10 plus s10 ipad air pro s4 s5 s6 s7 s8 lg g3 g4 g5 s6 s7 G3 G4 G5 samsung note 3 4 5 ✔️✔️✔️450 241-6313✔️✔️✔️ ...
 </t>
         </is>
       </c>
@@ -1606,14 +1605,14 @@
       <c r="A39" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Je paye $$$ pour tout IPHONE!
+                            RÉPARATION PROFESSIONNEL  DE VITRE SUR IPAD AIR 2 À100.00$ BAS PRIX !!! 514 947 1160
 </t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
           <t xml:space="preserve">
-         $1,000.00
+          Please Contact
                     </t>
         </is>
       </c>
@@ -1627,7 +1626,7 @@
       <c r="D39" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Je paye CASH sur le moment. je vien aussi cherche les telephones.! Iphone 8 Iphone 8 plus Iphone X Iphone XR Iphone XS Iphone XS MAX Iphone 11 Iphone 11 pro Iphone 11 pro max Tout les company sont accepte. Appel moi aujourd'hui pour un estimation. 514-465-6629 I Speak english also.
+                        Bonjour ! / Hi ! Nous offrons un service professionnel de réparation d'Iphone, Ipod et Ipad dans un délai plus que raisonnable ! Notre équipe de spécialistes fait aussi des réparations sur les téléphone LG tel que : LG G3 G4 G5 et plus encore. We offer a professional service for iphone, ipod and ipad repair with
 </t>
         </is>
       </c>
@@ -1636,29 +1635,29 @@
       <c r="A40" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            NEW SEALED IPHONE     11 64GB BLACK UNLOCKED
+                            OnePlus 8 PRO 12GB RAM 256GB BLACK IN2025 ✅ SEALED / SCELLÉ
 </t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $899.00
+                                    $1,099.00
                     </t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-Yesterday
+                            City of Montréal
+&lt; 37 minutes ago
 </t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        THIS LISTING IS FOR NEW SEA LED IPHONE 11 64GB BLACK UNLOCKED *************************************************************** BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA - ...
+                        OnePlus 8 Pro IN2025 BRAND NEW SEALED BOX WITH RECEIPT // NEUF DANS LA BOITE AVEC FACTURE ONYX BLACK COLOR • 120 Hz Fluid Display • Qualcomm® Snapdragon™ 865 and 5G • Warp Charge 30 Wireless • 48 MP ...
 </t>
         </is>
       </c>
@@ -1667,29 +1666,29 @@
       <c r="A41" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            NEW  IPHONE    11 64GB UNLOCKED BLK/RED/PURPLE
+                            10/10 iPhone 11 Pro Max 64GB - Unlocked
 </t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $899.00
+                                    $1,200.00
                     </t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-Yesterday
+                            City of Toronto
+&lt; 38 minutes ago
 </t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        THIS LISTING IS FOR NEW IPHONE 11 64GB UNLOCKED BLK/RED/PURPLE BUY FROM A STO RE BUY WITH CONFIDENCE BUYNCELL.CA ********************************************************************** VAUGHAN MILLS ...
+                        The phone is less than 2 weeks old and is in brand new condition with no scuffs or scratches anywhere on it It comes with the box and all original accessories It’s unlocked and will work with any ...
 </t>
         </is>
       </c>
@@ -1698,29 +1697,29 @@
       <c r="A42" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Brand new IPhone 11- Black 64gb
+                            iPhone Pro Max 11
 </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $900.00
+                                    $1,250.00
                     </t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Mississauga / Peel Region
-12/09/2020
+                            City of Toronto
+&lt; 39 minutes ago
 </t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Brand new purchased from Costco. Sealed in box.
+                        Brand new, in-box, sealed, iPhone Pro Max 11 Midnight Green. 64GB. $1250.00 Serious inquiries only. Low ball offers will be ignored.
 </t>
         </is>
       </c>
@@ -1729,29 +1728,29 @@
       <c r="A43" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Iphone 11 pro max 256 GB
+                            OnePlus 8 GLOW 12GB RAM 256GB BLACK IN2025 ✅ SEALED / SCELLÉ
 </t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,350.00
+                                    $940.00
                     </t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            City of Toronto
-02/09/2020
+                            City of Montréal
+&lt; 39 minutes ago
 </t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        10 /10 condition. New headphones never used. Comes with power adapter and charger , box. Thanks
+                        OnePlus 8 INTERSTELLAR GLOW IN2025 BRAND NEW SEALED BOX WITH RECEIPT // NEUF DANS LA BOITE AVEC FACTURE • 90 Hz Fluid Display • Qualcomm® Snapdragon™ 865 with 5G • Slim and Sleek Curved Design • 48 ...
 </t>
         </is>
       </c>
@@ -1760,29 +1759,29 @@
       <c r="A44" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 - New
+                            ✔️✅Répare ton Telephone brisé en 10min❤️✔️iPhone samsung lg iPad
 </t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $940.00
+                                    $39.00
                     </t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Ottawa
-12/09/2020
+                            City of Montréal
+&lt; 39 minutes ago
 </t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        iPhone 11 New 64gb. all in the accessories in the pictures are included and brand new. Price is Firm
+                        Iphone 7 water damage eau liquide carte mere motherboard lcd batterie battery 8 6s plus 11 pro max xs xr macbook pro huawei p30 5S 6S 7 X plus ipad air mini samsung s4 s5 s6 s7 s9 lg g3 g4 g5 note 10 ...
 </t>
         </is>
       </c>
@@ -1791,29 +1790,29 @@
       <c r="A45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            iPhone 11 Pro 64gig
+                            brand new iPhone XR
 </t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,100.00
+                                    $650.00
                     </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Calgary
-30/08/2020
+                            City of Toronto
+&lt; 40 minutes ago
 </t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        Only used for a month. Perfect condition. Comes with Otterbox case and ghost armour on both sides. Pick up in Capital Hill. Firm on price!
+                        brand new in box iPhone XR 64GB, comes with apple headphones and charger. Never used, got phone as a gift but already have the 11. Comes with a free screen protector.
 </t>
         </is>
       </c>
@@ -1822,29 +1821,29 @@
       <c r="A46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            BRAND NEW   SEALED IPHONE 11  PRO MAX (64GB) GOLD - $1449
+                            Apple i phone 11 asking $750 firm.
 </t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                                    $1,449.00
+                                     Please Contact
                     </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                            Markham / York Region
-12/09/2020
+                            Ottawa
+&lt; 40 minutes ago
 </t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
           <t xml:space="preserve">
-                        BRAND NEW SEALED IPHONE 11 PRO MAX (64GB) GOLD - $1449 Call us to reserve (905)850.0850 or email us your phone number. We are a store an d we are open as we are an essential business that do repair ...
+                        Great price for this phone unlocked.
 </t>
         </is>
       </c>

</xml_diff>